<commit_message>
Added example for `EchoProto.Templates.Loop_Assembly`
</commit_message>
<xml_diff>
--- a/Resources/For Docs/Labware_Layout_Files/Example DNA Stocks.xlsx
+++ b/Resources/For Docs/Labware_Layout_Files/Example DNA Stocks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b6068776_newcastle_ac_uk/Documents/Nextcloud/Private/Automation/AutomationResources/UserData/Bradle/Plate Layouts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/b6068776_newcastle_ac_uk/Documents/Nextcloud/Private/Automation/Automation_Protocols/BiomationScripter/Resources/For Docs/Labware_Layout_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{9C7C90C8-6531-4010-BBD1-5326B9149DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AA976CD-00FE-418D-B9E1-5164FA3E2B30}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{9C7C90C8-6531-4010-BBD1-5326B9149DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFE3E3F2-2EE4-40E5-8CF7-8AFF5A39D577}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="4176" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{9F5E6FB9-32EF-42A5-B114-36A33DEBE5EC}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="66">
   <si>
     <t>Plate Name</t>
   </si>
@@ -186,6 +186,72 @@
   </si>
   <si>
     <t>B0015</t>
+  </si>
+  <si>
+    <t>J23101</t>
+  </si>
+  <si>
+    <t>J23102</t>
+  </si>
+  <si>
+    <t>J23119</t>
+  </si>
+  <si>
+    <t>J23103</t>
+  </si>
+  <si>
+    <t>J23104</t>
+  </si>
+  <si>
+    <t>J23105</t>
+  </si>
+  <si>
+    <t>J23106</t>
+  </si>
+  <si>
+    <t>J23107</t>
+  </si>
+  <si>
+    <t>J23108</t>
+  </si>
+  <si>
+    <t>J23109</t>
+  </si>
+  <si>
+    <t>J23110</t>
+  </si>
+  <si>
+    <t>J23111</t>
+  </si>
+  <si>
+    <t>J23112</t>
+  </si>
+  <si>
+    <t>J23113</t>
+  </si>
+  <si>
+    <t>J23114</t>
+  </si>
+  <si>
+    <t>J23115</t>
+  </si>
+  <si>
+    <t>J23116</t>
+  </si>
+  <si>
+    <t>J23117</t>
+  </si>
+  <si>
+    <t>J23118</t>
+  </si>
+  <si>
+    <t>B0030</t>
+  </si>
+  <si>
+    <t>B0031</t>
+  </si>
+  <si>
+    <t>B0032</t>
   </si>
 </sst>
 </file>
@@ -644,7 +710,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -720,7 +786,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -741,7 +807,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E4">
         <v>50</v>
@@ -762,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>50</v>
@@ -783,7 +849,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <v>50</v>
@@ -804,7 +870,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <v>50</v>
@@ -824,6 +890,15 @@
       <c r="C8">
         <v>7</v>
       </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
@@ -836,6 +911,15 @@
       <c r="C9">
         <v>8</v>
       </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
@@ -848,6 +932,15 @@
       <c r="C10">
         <v>9</v>
       </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="I10" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
@@ -860,6 +953,15 @@
       <c r="C11">
         <v>10</v>
       </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
@@ -872,6 +974,15 @@
       <c r="C12">
         <v>11</v>
       </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
@@ -884,6 +995,15 @@
       <c r="C13">
         <v>12</v>
       </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
@@ -896,6 +1016,15 @@
       <c r="C14">
         <v>13</v>
       </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+      <c r="I14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
@@ -908,6 +1037,15 @@
       <c r="C15">
         <v>14</v>
       </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15">
+        <v>50</v>
+      </c>
+      <c r="I15" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
@@ -920,8 +1058,17 @@
       <c r="C16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+      <c r="I16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>A16</v>
@@ -932,8 +1079,17 @@
       <c r="C17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17">
+        <v>50</v>
+      </c>
+      <c r="I17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>A17</v>
@@ -944,8 +1100,17 @@
       <c r="C18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <v>50</v>
+      </c>
+      <c r="I18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>A18</v>
@@ -956,8 +1121,17 @@
       <c r="C19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19">
+        <v>50</v>
+      </c>
+      <c r="I19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>A19</v>
@@ -968,8 +1142,17 @@
       <c r="C20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20">
+        <v>50</v>
+      </c>
+      <c r="I20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>A20</v>
@@ -980,8 +1163,17 @@
       <c r="C21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="I21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>A21</v>
@@ -992,8 +1184,17 @@
       <c r="C22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22">
+        <v>50</v>
+      </c>
+      <c r="I22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>A22</v>
@@ -1004,8 +1205,17 @@
       <c r="C23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23">
+        <v>50</v>
+      </c>
+      <c r="I23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>A23</v>
@@ -1016,8 +1226,17 @@
       <c r="C24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24">
+        <v>50</v>
+      </c>
+      <c r="I24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>A24</v>
@@ -1028,8 +1247,17 @@
       <c r="C25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25">
+        <v>50</v>
+      </c>
+      <c r="I25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>B1</v>
@@ -1040,8 +1268,17 @@
       <c r="C26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26">
+        <v>50</v>
+      </c>
+      <c r="I26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>B2</v>
@@ -1052,8 +1289,17 @@
       <c r="C27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27">
+        <v>50</v>
+      </c>
+      <c r="I27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>B3</v>
@@ -1064,8 +1310,17 @@
       <c r="C28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28">
+        <v>50</v>
+      </c>
+      <c r="I28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>B4</v>
@@ -1076,8 +1331,17 @@
       <c r="C29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29">
+        <v>50</v>
+      </c>
+      <c r="I29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>B5</v>
@@ -1088,8 +1352,17 @@
       <c r="C30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30">
+        <v>50</v>
+      </c>
+      <c r="I30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>B6</v>
@@ -1100,8 +1373,17 @@
       <c r="C31">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31">
+        <v>50</v>
+      </c>
+      <c r="I31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>B7</v>
@@ -1112,8 +1394,17 @@
       <c r="C32">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32">
+        <v>50</v>
+      </c>
+      <c r="I32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>B8</v>
@@ -1124,8 +1415,17 @@
       <c r="C33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33">
+        <v>50</v>
+      </c>
+      <c r="I33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>B9</v>
@@ -1136,8 +1436,17 @@
       <c r="C34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34">
+        <v>50</v>
+      </c>
+      <c r="I34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>B10</v>
@@ -1148,8 +1457,17 @@
       <c r="C35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E35">
+        <v>50</v>
+      </c>
+      <c r="I35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>B11</v>
@@ -1160,8 +1478,17 @@
       <c r="C36">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36">
+        <v>50</v>
+      </c>
+      <c r="I36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>B12</v>
@@ -1172,8 +1499,17 @@
       <c r="C37">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37">
+        <v>50</v>
+      </c>
+      <c r="I37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>B13</v>
@@ -1185,7 +1521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>B14</v>
@@ -1197,7 +1533,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>B15</v>
@@ -1209,7 +1545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>B16</v>
@@ -1221,7 +1557,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>B17</v>
@@ -1233,7 +1569,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>B18</v>
@@ -1245,7 +1581,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>B19</v>
@@ -1257,7 +1593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>B20</v>
@@ -1269,7 +1605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>B21</v>
@@ -1281,7 +1617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>B22</v>
@@ -1293,7 +1629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>B23</v>

</xml_diff>